<commit_message>
fine tuning the summary story
</commit_message>
<xml_diff>
--- a/templates/Solver Optimizer.xlsx
+++ b/templates/Solver Optimizer.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>ProblemID</t>
   </si>
@@ -280,13 +280,364 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Summary: Utilizing 100% of allocated budget, we could unlock 53% impact value problems using manual weighted normalization calc method.</t>
-  </si>
-  <si>
-    <t>Summary: Utilizing 90% of allocated budget, we could unlock 57% impact value problems using winsorized MIN-MAX normalization cal method.</t>
-  </si>
-  <si>
     <t>manual weighted normalization calc based on data analytics</t>
+  </si>
+  <si>
+    <t>Hrs Used</t>
+  </si>
+  <si>
+    <t>ImpactScore Solved</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Summary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: By utilizing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the allocated budget, we can unlock </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>57%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the impact value from the PB backlog using the Winsorized Min-Max normalization calculation method</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Storyline Summary:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If we had prioritized instinct or highest impact items, we might have selected </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PRB003.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> However, this option would have consumed 150 hrs, ie </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>75%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the total budget while only addressing</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 39%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the backlog impact, which is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>18% lower</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">than the solver’s recommendation. Even by adding PRB002 for the remaining 40 hours, the total effort would use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>95%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the budget to achieve</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 47% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of the backlog impact still 10% less effective than the optimizer’s solution which is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> utilization to address</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 57%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> impact value still leaving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>buffer of 10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> budget in hand.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Summary: By utilizatin </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of allocated budget, we can unlock </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>53%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> impact value from the PB backlog using manual weighted normalization method.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -296,7 +647,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +673,36 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,7 +740,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -494,20 +875,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -544,15 +916,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -586,32 +949,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -626,72 +993,23 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Curved Connector 1"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="6407150" y="1981200"/>
-          <a:ext cx="1727200" cy="774700"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -15809"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>885601</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>340810</xdr:rowOff>
+      <xdr:colOff>109368</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>175994</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3086550" cy="937629"/>
+    <xdr:ext cx="4639027" cy="530658"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="20686726">
-          <a:off x="1552351" y="2734760"/>
-          <a:ext cx="3086550" cy="937629"/>
+        <a:xfrm rot="21024607">
+          <a:off x="776118" y="6075144"/>
+          <a:ext cx="4639027" cy="530658"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -706,7 +1024,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="5400" b="0" cap="none" spc="0">
+            <a:rPr lang="en-US" sz="2800" b="0" cap="none" spc="0">
               <a:ln w="0"/>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -719,7 +1037,39 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>Eg. for Ref</a:t>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> calc steps are </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>for Ref Only</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -992,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,14 +1360,15 @@
     <col min="8" max="8" width="7.26953125" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" customWidth="1"/>
     <col min="12" max="12" width="9.08984375" customWidth="1"/>
     <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
+    <col min="16" max="16" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1053,10 +1404,10 @@
       </c>
       <c r="L1" s="9"/>
       <c r="M1" s="9" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>16</v>
@@ -1064,10 +1415,10 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="13">
@@ -1082,23 +1433,23 @@
       <c r="F2" s="13">
         <v>80</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="22">
         <f>(MIN(MAX(C2, (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))), (_xlfn.PERCENTILE.INC(C$2:C$7, 0.95))) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))) / ((_xlfn.PERCENTILE.INC(C$2:C$7, 0.95)) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05)))</f>
         <v>0.62790697674418605</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="22">
         <f>(MIN(MAX(D2, (_xlfn.PERCENTILE.INC(D$2:D$7, 0.05))), (_xlfn.PERCENTILE.INC(D$2:D$7, 0.95))) - (_xlfn.PERCENTILE.INC(D$2:D$7, 0.05))) / ((_xlfn.PERCENTILE.INC(D$2:D$7, 0.95)) - (_xlfn.PERCENTILE.INC(D$2:D$7, 0.05)))</f>
         <v>0.34040047114252059</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="22">
         <f>(MIN(MAX(E2, (_xlfn.PERCENTILE.INC(E$2:E$7, 0.05))), (_xlfn.PERCENTILE.INC(E$2:E$7, 0.95))) - (_xlfn.PERCENTILE.INC(E$2:E$7, 0.05))) / ((_xlfn.PERCENTILE.INC(E$2:E$7, 0.95)) - (_xlfn.PERCENTILE.INC(E$2:E$7, 0.05)))</f>
         <v>0.73913043478260865</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="23">
         <f>SUM(G2:I2)</f>
         <v>1.7074378826693153</v>
       </c>
-      <c r="K2" s="27">
+      <c r="K2" s="24">
         <v>1</v>
       </c>
       <c r="L2" s="2"/>
@@ -1110,16 +1461,16 @@
         <f>SUMPRODUCT(F2:F7, K2:K7)</f>
         <v>180</v>
       </c>
-      <c r="O2" s="28">
+      <c r="O2" s="25">
         <v>200</v>
       </c>
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="13">
@@ -1134,23 +1485,23 @@
       <c r="F3" s="13">
         <v>40</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <f t="shared" ref="G3:I7" si="0">(MIN(MAX(C3, (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))), (_xlfn.PERCENTILE.INC(C$2:C$7, 0.95))) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))) / ((_xlfn.PERCENTILE.INC(C$2:C$7, 0.95)) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05)))</f>
         <v>0.16279069767441862</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="22">
         <f t="shared" si="0"/>
         <v>5.7714958775029447E-2</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="22">
         <f t="shared" si="0"/>
         <v>0.36231884057971014</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="23">
         <f t="shared" ref="J3:J7" si="1">SUM(G3:I3)</f>
         <v>0.58282449702915817</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="24">
         <v>1</v>
       </c>
       <c r="L3" s="2"/>
@@ -1158,7 +1509,7 @@
         <f>M2/J9</f>
         <v>0.57203210560330664</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="34">
         <f>N2/O2</f>
         <v>0.9</v>
       </c>
@@ -1166,10 +1517,10 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="13">
@@ -1184,23 +1535,23 @@
       <c r="F4" s="13">
         <v>150</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="22">
         <f t="shared" si="0"/>
         <v>0.9130434782608694</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="23">
         <f t="shared" si="1"/>
         <v>2.9130434782608692</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="24">
         <v>0</v>
       </c>
       <c r="L4" s="2"/>
@@ -1209,11 +1560,11 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="13">
@@ -1228,38 +1579,38 @@
       <c r="F5" s="13">
         <v>60</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>0.37984496124031009</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="22">
         <f t="shared" si="0"/>
         <v>0.5053003533568905</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="23">
         <f t="shared" si="1"/>
         <v>1.8851453145972006</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="24">
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
+      <c r="M5" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="13">
@@ -1274,36 +1625,36 @@
       <c r="F6" s="13">
         <v>25</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>6.9767441860465115E-2</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <f t="shared" si="0"/>
         <v>1.0600706713780919E-2</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="22">
         <f t="shared" si="0"/>
         <v>0.1304347826086957</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="23">
         <f t="shared" si="1"/>
         <v>0.21080293118294174</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="24">
         <v>0</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="13">
@@ -1318,30 +1669,30 @@
       <c r="F7" s="13">
         <v>35</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="24">
         <v>0</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
@@ -1354,10 +1705,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
@@ -1366,7 +1717,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="J9" s="4">
         <f>SUM(J2:J7)</f>
         <v>7.2992541037394849</v>
@@ -1378,247 +1731,331 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K10" s="33"/>
+    </row>
+    <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+    </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+    </row>
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H20" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="19">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="16">
         <v>75000</v>
       </c>
-      <c r="B14" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.05)</f>
+      <c r="B21" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
-      <c r="C14" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.95)</f>
+      <c r="C21" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
-      <c r="D14" s="13">
-        <f>MAX(A14,B14)</f>
+      <c r="D21" s="13">
+        <f>MAX(A21,B21)</f>
         <v>75000</v>
       </c>
-      <c r="E14" s="13">
-        <f>MIN(D14,C14)</f>
+      <c r="E21" s="13">
+        <f>MIN(D21,C21)</f>
         <v>75000</v>
       </c>
-      <c r="F14" s="13">
-        <f>E14-B14</f>
+      <c r="F21" s="13">
+        <f>E21-B21</f>
         <v>72250</v>
       </c>
-      <c r="G14" s="13">
-        <f>C14-B14</f>
+      <c r="G21" s="13">
+        <f>C21-B21</f>
         <v>212250</v>
       </c>
-      <c r="H14" s="20">
-        <f>F14/G14</f>
+      <c r="H21" s="17">
+        <f>F21/G21</f>
         <v>0.34040047114252059</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="19">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="16">
         <v>15000</v>
       </c>
-      <c r="B15" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.05)</f>
+      <c r="B22" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
-      <c r="C15" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.95)</f>
+      <c r="C22" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
-      <c r="D15" s="13">
-        <f t="shared" ref="D15:D19" si="2">MAX(A15,B15)</f>
+      <c r="D22" s="13">
+        <f t="shared" ref="D22:D26" si="2">MAX(A22,B22)</f>
         <v>15000</v>
       </c>
-      <c r="E15" s="13">
-        <f t="shared" ref="E15:E19" si="3">MIN(D15,C15)</f>
+      <c r="E22" s="13">
+        <f t="shared" ref="E22:E26" si="3">MIN(D22,C22)</f>
         <v>15000</v>
       </c>
-      <c r="F15" s="13">
-        <f t="shared" ref="F15:F19" si="4">E15-B15</f>
+      <c r="F22" s="13">
+        <f t="shared" ref="F22:F26" si="4">E22-B22</f>
         <v>12250</v>
       </c>
-      <c r="G15" s="13">
-        <f t="shared" ref="G15:G19" si="5">C15-B15</f>
+      <c r="G22" s="13">
+        <f t="shared" ref="G22:G26" si="5">C22-B22</f>
         <v>212250</v>
       </c>
-      <c r="H15" s="20">
-        <f t="shared" ref="H15:H19" si="6">F15/G15</f>
+      <c r="H22" s="17">
+        <f t="shared" ref="H22:H26" si="6">F22/G22</f>
         <v>5.7714958775029447E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="19">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="16">
         <v>250000</v>
       </c>
-      <c r="B16" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.05)</f>
+      <c r="B23" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
-      <c r="C16" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.95)</f>
+      <c r="C23" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D23" s="13">
         <f t="shared" si="2"/>
         <v>250000</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E23" s="13">
         <f t="shared" si="3"/>
         <v>215000</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F23" s="13">
         <f t="shared" si="4"/>
         <v>212250</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G23" s="13">
         <f t="shared" si="5"/>
         <v>212250</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H23" s="17">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="19">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="16">
         <v>110000</v>
       </c>
-      <c r="B17" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.05)</f>
+      <c r="B24" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
-      <c r="C17" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.95)</f>
+      <c r="C24" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D24" s="13">
         <f t="shared" si="2"/>
         <v>110000</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E24" s="13">
         <f t="shared" si="3"/>
         <v>110000</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F24" s="13">
         <f t="shared" si="4"/>
         <v>107250</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G24" s="13">
         <f t="shared" si="5"/>
         <v>212250</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H24" s="17">
         <f t="shared" si="6"/>
         <v>0.5053003533568905</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="19">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="16">
         <v>5000</v>
       </c>
-      <c r="B18" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.05)</f>
+      <c r="B25" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
-      <c r="C18" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.95)</f>
+      <c r="C25" s="13">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D25" s="13">
         <f t="shared" si="2"/>
         <v>5000</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E25" s="13">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F25" s="13">
         <f t="shared" si="4"/>
         <v>2250</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G25" s="13">
         <f t="shared" si="5"/>
         <v>212250</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H25" s="17">
         <f t="shared" si="6"/>
         <v>1.0600706713780919E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="21">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="18">
         <v>2000</v>
       </c>
-      <c r="B19" s="22">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.05)</f>
+      <c r="B26" s="19">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
-      <c r="C19" s="22">
-        <f>_xlfn.PERCENTILE.INC($A$14:$A$19, 0.95)</f>
+      <c r="C26" s="19">
+        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D26" s="19">
         <f t="shared" si="2"/>
         <v>2750</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E26" s="19">
         <f t="shared" si="3"/>
         <v>2750</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F26" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G26" s="19">
         <f t="shared" si="5"/>
         <v>212250</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H26" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A12:H12"/>
+  <mergeCells count="3">
+    <mergeCell ref="A19:H19"/>
     <mergeCell ref="M5:P8"/>
+    <mergeCell ref="A11:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1631,7 +2068,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1700,10 +2137,10 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="13">
@@ -1718,23 +2155,23 @@
       <c r="F2" s="13">
         <v>80</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="22">
         <f>C2*0.1</f>
         <v>12</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="22">
         <f>D2/1000</f>
         <v>75</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="22">
         <f>E2*10</f>
         <v>85</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="23">
         <f>SUM(G2:I2)</f>
         <v>172</v>
       </c>
-      <c r="K2" s="27">
+      <c r="K2" s="24">
         <v>1</v>
       </c>
       <c r="L2" s="2"/>
@@ -1746,16 +2183,16 @@
         <f>SUMPRODUCT(F2:F7, K2:K7)</f>
         <v>200</v>
       </c>
-      <c r="O2" s="28">
+      <c r="O2" s="25">
         <v>200</v>
       </c>
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="13">
@@ -1770,23 +2207,23 @@
       <c r="F3" s="13">
         <v>40</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <f t="shared" ref="G3:G7" si="0">C3*0.1</f>
         <v>4.5</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="22">
         <f t="shared" ref="H3:H7" si="1">D3/1000</f>
         <v>15</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="22">
         <f t="shared" ref="I3:I7" si="2">E3*10</f>
         <v>72</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="23">
         <f t="shared" ref="J3:J7" si="3">SUM(G3:I3)</f>
         <v>91.5</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="24">
         <v>0</v>
       </c>
       <c r="L3" s="2"/>
@@ -1802,10 +2239,10 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="13">
@@ -1820,23 +2257,23 @@
       <c r="F4" s="13">
         <v>150</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="22">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="22">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="23">
         <f t="shared" si="3"/>
         <v>361</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="24">
         <v>0</v>
       </c>
       <c r="L4" s="2"/>
@@ -1846,10 +2283,10 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="13">
@@ -1864,38 +2301,38 @@
       <c r="F5" s="13">
         <v>60</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="22">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="22">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="23">
         <f t="shared" si="3"/>
         <v>213</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="24">
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
+      <c r="M5" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="13">
@@ -1910,36 +2347,36 @@
       <c r="F6" s="13">
         <v>25</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="22">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="23">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="24">
         <v>1</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="13">
@@ -1954,30 +2391,30 @@
       <c r="F7" s="13">
         <v>35</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="22">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="22">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="23">
         <f t="shared" si="3"/>
         <v>61.5</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="24">
         <v>1</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
@@ -1990,10 +2427,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
@@ -2018,7 +2455,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
2 sheets for optimizer model comparison
</commit_message>
<xml_diff>
--- a/templates/Solver Optimizer.xlsx
+++ b/templates/Solver Optimizer.xlsx
@@ -298,74 +298,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Summary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: By utilizing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>90%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the allocated budget, we can unlock </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>57%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the impact value from the PB backlog using the Winsorized Min-Max normalization calculation method</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Storyline Summary:</t>
     </r>
     <r>
@@ -637,6 +569,74 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> impact value from the PB backlog using manual weighted normalization method.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Summary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: By utilizing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the allocated budget, we can unlock </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>57%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the impact value from the PB backlog using the Winsorized Min-Max normalization calculation method.</t>
     </r>
   </si>
 </sst>
@@ -949,29 +949,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1345,7 +1345,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1509,7 +1509,7 @@
         <f>M2/J9</f>
         <v>0.57203210560330664</v>
       </c>
-      <c r="N3" s="34">
+      <c r="N3" s="28">
         <f>N2/O2</f>
         <v>0.9</v>
       </c>
@@ -1560,7 +1560,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
@@ -1599,12 +1599,12 @@
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="M5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
@@ -1645,10 +1645,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
@@ -1689,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
@@ -1705,10 +1705,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
@@ -1726,106 +1726,106 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K10" s="33"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="A11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
@@ -1858,11 +1858,11 @@
         <v>75000</v>
       </c>
       <c r="B21" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
+        <f t="shared" ref="B21:B26" si="2">_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
         <v>2750</v>
       </c>
       <c r="C21" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
+        <f t="shared" ref="C21:C26" si="3">_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
         <v>215000</v>
       </c>
       <c r="D21" s="13">
@@ -1891,31 +1891,31 @@
         <v>15000</v>
       </c>
       <c r="B22" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
+        <f t="shared" si="2"/>
         <v>2750</v>
       </c>
       <c r="C22" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
+        <f t="shared" si="3"/>
         <v>215000</v>
       </c>
       <c r="D22" s="13">
-        <f t="shared" ref="D22:D26" si="2">MAX(A22,B22)</f>
+        <f t="shared" ref="D22:D26" si="4">MAX(A22,B22)</f>
         <v>15000</v>
       </c>
       <c r="E22" s="13">
-        <f t="shared" ref="E22:E26" si="3">MIN(D22,C22)</f>
+        <f t="shared" ref="E22:E26" si="5">MIN(D22,C22)</f>
         <v>15000</v>
       </c>
       <c r="F22" s="13">
-        <f t="shared" ref="F22:F26" si="4">E22-B22</f>
+        <f t="shared" ref="F22:F26" si="6">E22-B22</f>
         <v>12250</v>
       </c>
       <c r="G22" s="13">
-        <f t="shared" ref="G22:G26" si="5">C22-B22</f>
+        <f t="shared" ref="G22:G26" si="7">C22-B22</f>
         <v>212250</v>
       </c>
       <c r="H22" s="17">
-        <f t="shared" ref="H22:H26" si="6">F22/G22</f>
+        <f t="shared" ref="H22:H26" si="8">F22/G22</f>
         <v>5.7714958775029447E-2</v>
       </c>
     </row>
@@ -1924,31 +1924,31 @@
         <v>250000</v>
       </c>
       <c r="B23" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
+        <f t="shared" si="2"/>
         <v>2750</v>
       </c>
       <c r="C23" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
-        <v>215000</v>
-      </c>
-      <c r="D23" s="13">
-        <f t="shared" si="2"/>
-        <v>250000</v>
-      </c>
-      <c r="E23" s="13">
         <f t="shared" si="3"/>
         <v>215000</v>
       </c>
+      <c r="D23" s="13">
+        <f t="shared" si="4"/>
+        <v>250000</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="5"/>
+        <v>215000</v>
+      </c>
       <c r="F23" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>212250</v>
       </c>
       <c r="G23" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>212250</v>
       </c>
       <c r="H23" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -1957,31 +1957,31 @@
         <v>110000</v>
       </c>
       <c r="B24" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
+        <f t="shared" si="2"/>
         <v>2750</v>
       </c>
       <c r="C24" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
+        <f t="shared" si="3"/>
         <v>215000</v>
       </c>
       <c r="D24" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>110000</v>
       </c>
       <c r="E24" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>110000</v>
       </c>
       <c r="F24" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>107250</v>
       </c>
       <c r="G24" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>212250</v>
       </c>
       <c r="H24" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5053003533568905</v>
       </c>
     </row>
@@ -1990,31 +1990,31 @@
         <v>5000</v>
       </c>
       <c r="B25" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
+        <f t="shared" si="2"/>
         <v>2750</v>
       </c>
       <c r="C25" s="13">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
+        <f t="shared" si="3"/>
         <v>215000</v>
       </c>
       <c r="D25" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="E25" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5000</v>
       </c>
       <c r="F25" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2250</v>
       </c>
       <c r="G25" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>212250</v>
       </c>
       <c r="H25" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.0600706713780919E-2</v>
       </c>
     </row>
@@ -2023,39 +2023,39 @@
         <v>2000</v>
       </c>
       <c r="B26" s="19">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.05)</f>
-        <v>2750</v>
-      </c>
-      <c r="C26" s="19">
-        <f>_xlfn.PERCENTILE.INC($A$21:$A$26, 0.95)</f>
-        <v>215000</v>
-      </c>
-      <c r="D26" s="19">
         <f t="shared" si="2"/>
         <v>2750</v>
       </c>
+      <c r="C26" s="19">
+        <f t="shared" si="3"/>
+        <v>215000</v>
+      </c>
+      <c r="D26" s="19">
+        <f t="shared" si="4"/>
+        <v>2750</v>
+      </c>
       <c r="E26" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2750</v>
       </c>
       <c r="F26" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G26" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>212250</v>
       </c>
       <c r="H26" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="M5:P8"/>
     <mergeCell ref="A11:K15"/>
+    <mergeCell ref="M5:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2321,12 +2321,12 @@
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="M5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
@@ -2367,10 +2367,10 @@
         <v>1</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
@@ -2411,10 +2411,10 @@
         <v>1</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
@@ -2427,10 +2427,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>

</xml_diff>

<commit_message>
2 sheets to compare optimizer model results
</commit_message>
<xml_diff>
--- a/templates/Solver Optimizer.xlsx
+++ b/templates/Solver Optimizer.xlsx
@@ -290,6 +290,9 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Summary: By utilizatin </t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -298,6 +301,142 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>100%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of allocated budget, we can unlock </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>53%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> impact value from the PB backlog using manual weighted normalization method.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Summary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: By utilizing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the allocated budget, we can unlock </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>57%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the impact value and still leaving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> buffer on budget using the Winsorized Min-Max normalization model.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Storyline Summary:</t>
     </r>
     <r>
@@ -309,7 +448,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-If we had prioritized instinct or highest impact items, we might have selected </t>
+If we had prioritized with instinct gut feeling or literally highest impact items, we might have selected </t>
     </r>
     <r>
       <rPr>
@@ -341,7 +480,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>75%</t>
+      <t>82%</t>
     </r>
     <r>
       <rPr>
@@ -414,18 +553,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">than the solver’s recommendation. Even by adding PRB002 for the remaining 40 hours, the total effort would use </t>
+      <t xml:space="preserve">than the optimizer’s recommended solution which is </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>95%</t>
+      <t xml:space="preserve"> utilization to address</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 57%</t>
     </r>
     <r>
       <rPr>
@@ -435,208 +595,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> of the budget to achieve</t>
+      <t xml:space="preserve"> impact value, still leaving a </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 47% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">of the backlog impact still 10% less effective than the optimizer’s solution which is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>90%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> utilization to address</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 57%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> impact value still leaving </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>buffer of 10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> budget in hand.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Summary: By utilizatin </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>100%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of allocated budget, we can unlock </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>53%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> impact value from the PB backlog using manual weighted normalization method.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Summary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: By utilizing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>90%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the allocated budget, we can unlock </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>57%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the impact value from the PB backlog using the Winsorized Min-Max normalization calculation method.</t>
+      <t xml:space="preserve"> buffer on the budget.</t>
     </r>
   </si>
 </sst>
@@ -879,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -965,15 +945,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1345,7 +1326,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1533,7 +1514,7 @@
         <v>9.1</v>
       </c>
       <c r="F4" s="13">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G4" s="22">
         <f t="shared" si="0"/>
@@ -1599,12 +1580,12 @@
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
+      <c r="M5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
@@ -1645,10 +1626,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
@@ -1689,10 +1670,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
@@ -1705,10 +1686,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
@@ -1726,80 +1707,80 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
+      <c r="A11" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="29"/>
@@ -2068,7 +2049,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2189,7 +2170,7 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -2255,7 +2236,7 @@
         <v>9.1</v>
       </c>
       <c r="F4" s="13">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G4" s="22">
         <f t="shared" si="0"/>
@@ -2321,15 +2302,15 @@
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
+      <c r="M5" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -2367,13 +2348,13 @@
         <v>1</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -2411,10 +2392,10 @@
         <v>1</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
@@ -2427,10 +2408,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>

</xml_diff>

<commit_message>
infographic added in model result page
</commit_message>
<xml_diff>
--- a/templates/Solver Optimizer.xlsx
+++ b/templates/Solver Optimizer.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>ProblemID</t>
   </si>
@@ -338,6 +338,12 @@
     </r>
   </si>
   <si>
+    <t>Gut feel = 2.9 impact score (39% impact solved)</t>
+  </si>
+  <si>
+    <t>Optimizer = 4.2 impact score (57% impact solved)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -347,97 +353,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Summary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: By utilizing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>100%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the allocated budget, we can unlock </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>57%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the impact value and still leaving </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> buffer on budget using the Winsorized Min-Max normalization model.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Storyline Summary:</t>
+      <t xml:space="preserve">                                                                                                   Storyline Summary:</t>
     </r>
     <r>
       <rPr>
@@ -469,7 +385,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> However, this option would have consumed 150 hrs, ie </t>
+      <t xml:space="preserve"> However, this option would have consumed 165 hrs, ie </t>
     </r>
     <r>
       <rPr>
@@ -574,7 +490,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> utilization to address</t>
+      <t xml:space="preserve"> utilization of budget to address</t>
     </r>
     <r>
       <rPr>
@@ -616,7 +532,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> buffer on the budget.</t>
+      <t xml:space="preserve"> buffer in budget.</t>
     </r>
   </si>
 </sst>
@@ -627,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,8 +603,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -716,6 +640,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -936,6 +878,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -948,13 +891,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,6 +921,1103 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'winsorized Min–Max norm'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ImpactScore</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-14F8-4AEF-8A26-12A37B50675C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-14F8-4AEF-8A26-12A37B50675C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-14F8-4AEF-8A26-12A37B50675C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-14F8-4AEF-8A26-12A37B50675C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-14F8-4AEF-8A26-12A37B50675C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'winsorized Min–Max norm'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>PRB001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PRB002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PRB003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PRB004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>PRB005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>PRB006</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'winsorized Min–Max norm'!$J$2:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.7074378826693153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58282449702915817</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9130434782608692</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8851453145972006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21080293118294174</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-14F8-4AEF-8A26-12A37B50675C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="65"/>
+        <c:axId val="488763416"/>
+        <c:axId val="488762104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="488763416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488762104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488762104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="488763416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1057,6 +2105,36 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1323,25 +2401,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" customWidth="1"/>
     <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.26953125" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.08984375" customWidth="1"/>
     <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.453125" bestFit="1" customWidth="1"/>
@@ -1349,7 +2427,7 @@
     <col min="16" max="16" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +2473,7 @@
       </c>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
@@ -1414,15 +2492,15 @@
       <c r="F2" s="13">
         <v>80</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="37">
         <f>(MIN(MAX(C2, (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))), (_xlfn.PERCENTILE.INC(C$2:C$7, 0.95))) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))) / ((_xlfn.PERCENTILE.INC(C$2:C$7, 0.95)) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05)))</f>
         <v>0.62790697674418605</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="37">
         <f>(MIN(MAX(D2, (_xlfn.PERCENTILE.INC(D$2:D$7, 0.05))), (_xlfn.PERCENTILE.INC(D$2:D$7, 0.95))) - (_xlfn.PERCENTILE.INC(D$2:D$7, 0.05))) / ((_xlfn.PERCENTILE.INC(D$2:D$7, 0.95)) - (_xlfn.PERCENTILE.INC(D$2:D$7, 0.05)))</f>
         <v>0.34040047114252059</v>
       </c>
-      <c r="I2" s="22">
+      <c r="I2" s="37">
         <f>(MIN(MAX(E2, (_xlfn.PERCENTILE.INC(E$2:E$7, 0.05))), (_xlfn.PERCENTILE.INC(E$2:E$7, 0.95))) - (_xlfn.PERCENTILE.INC(E$2:E$7, 0.05))) / ((_xlfn.PERCENTILE.INC(E$2:E$7, 0.95)) - (_xlfn.PERCENTILE.INC(E$2:E$7, 0.05)))</f>
         <v>0.73913043478260865</v>
       </c>
@@ -1447,7 +2525,7 @@
       </c>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
@@ -1466,15 +2544,15 @@
       <c r="F3" s="13">
         <v>40</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="37">
         <f t="shared" ref="G3:I7" si="0">(MIN(MAX(C3, (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))), (_xlfn.PERCENTILE.INC(C$2:C$7, 0.95))) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05))) / ((_xlfn.PERCENTILE.INC(C$2:C$7, 0.95)) - (_xlfn.PERCENTILE.INC(C$2:C$7, 0.05)))</f>
         <v>0.16279069767441862</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="37">
         <f t="shared" si="0"/>
         <v>5.7714958775029447E-2</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="37">
         <f t="shared" si="0"/>
         <v>0.36231884057971014</v>
       </c>
@@ -1497,7 +2575,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
@@ -1516,15 +2594,15 @@
       <c r="F4" s="13">
         <v>165</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="37">
         <f t="shared" si="0"/>
         <v>0.9130434782608694</v>
       </c>
@@ -1541,7 +2619,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
@@ -1560,15 +2638,15 @@
       <c r="F5" s="13">
         <v>60</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="37">
         <f t="shared" si="0"/>
         <v>0.37984496124031009</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="37">
         <f t="shared" si="0"/>
         <v>0.5053003533568905</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="37">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1580,14 +2658,12 @@
         <v>1</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>11</v>
       </c>
@@ -1606,15 +2682,15 @@
       <c r="F6" s="13">
         <v>25</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="37">
         <f t="shared" si="0"/>
         <v>6.9767441860465115E-2</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="37">
         <f t="shared" si="0"/>
         <v>1.0600706713780919E-2</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="37">
         <f t="shared" si="0"/>
         <v>0.1304347826086957</v>
       </c>
@@ -1626,12 +2702,12 @@
         <v>0</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
@@ -1650,15 +2726,15 @@
       <c r="F7" s="13">
         <v>35</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1670,12 +2746,12 @@
         <v>0</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1686,12 +2762,12 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1707,82 +2783,96 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="K10" s="27"/>
     </row>
-    <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="33" t="s">
+    <row r="11" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="M14" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="M15" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="29"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -1797,16 +2887,16 @@
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
@@ -2033,10 +3123,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A11:K15"/>
-    <mergeCell ref="M5:P9"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2310,7 +3401,7 @@
       <c r="P5" s="35"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -2354,7 +3445,7 @@
       <c r="P6" s="35"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="21" t="s">

</xml_diff>